<commit_message>
fixed errors related to scrapping
</commit_message>
<xml_diff>
--- a/build/exe.win-amd64-3.8/suivi.xlsx
+++ b/build/exe.win-amd64-3.8/suivi.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiphaine\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\olivier\ballon d'eau\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104B9560-DAD0-45F4-8455-76AB429B2597}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A2746E6-4405-4334-AC9D-601E60E8E466}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{C411A034-5389-4F96-8ECE-DDB492652C9E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C411A034-5389-4F96-8ECE-DDB492652C9E}"/>
   </bookViews>
   <sheets>
     <sheet name="produits à surveiller" sheetId="2" r:id="rId1"/>
     <sheet name="cdes et cout" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'produits à surveiller'!$A$1:$S$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'produits à surveiller'!$A$1:$S$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="496">
   <si>
     <t>154330-l</t>
   </si>
@@ -1451,6 +1451,24 @@
   </si>
   <si>
     <t>022330-L</t>
+  </si>
+  <si>
+    <t>https://www.eau-go.fr/3294-thickbox_default/chauffe-eau-electrique-200l-atlantic-chauffeo-vertical-sur-socle.jpg</t>
+  </si>
+  <si>
+    <t>https://www.eau-go.fr/chauffe-eau-electrique-200l-atlantic-chauffeo-vertical-sur-socle-46.html</t>
+  </si>
+  <si>
+    <t>411.00 €</t>
+  </si>
+  <si>
+    <t>Ce chauffe eau électrique vertical d'une capacité de 200 litres est issu de la gamme Chaufféo du fabricant français Atlantic. Ce ballon d'eau chaude est idéal pour répondre aux besoins en eau chaude sanitaire de 4 personnes</t>
+  </si>
+  <si>
+    <t>Chauffe-eau électrique 200L ATLANTIC Chauffeo vertical sur socle</t>
+  </si>
+  <si>
+    <t>022120-L</t>
   </si>
   <si>
     <t>custom_label_0</t>
@@ -1986,84 +2004,84 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA999"/>
+  <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I19" workbookViewId="0">
-      <selection activeCell="I27" sqref="A27:XFD27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="14.41796875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="72.578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="66.83984375" style="6" customWidth="1"/>
-    <col min="5" max="7" width="14.41796875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="80.26171875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="113.83984375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="21.41796875" style="16" customWidth="1"/>
-    <col min="11" max="17" width="14.41796875" style="6"/>
+    <col min="1" max="2" width="14.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="72.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="66.85546875" style="6" customWidth="1"/>
+    <col min="5" max="7" width="14.42578125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="80.28515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="113.85546875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" style="16" customWidth="1"/>
+    <col min="11" max="17" width="14.42578125" style="6"/>
     <col min="18" max="18" width="25" style="6" customWidth="1"/>
-    <col min="19" max="27" width="35.83984375" style="6" customWidth="1"/>
-    <col min="28" max="16384" width="14.41796875" style="6"/>
+    <col min="19" max="27" width="35.85546875" style="6" customWidth="1"/>
+    <col min="28" max="16384" width="14.42578125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1" s="14" t="s">
+        <v>494</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>495</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>493</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>492</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>490</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>489</v>
+      </c>
+      <c r="H1" s="14" t="s">
         <v>488</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>489</v>
-      </c>
-      <c r="C1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>487</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="J1" s="15" t="s">
         <v>486</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>485</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>483</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>481</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="P1" s="13" t="s">
         <v>480</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="Q1" s="12" t="s">
         <v>479</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="R1" s="12" t="s">
         <v>478</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="S1" s="12" t="s">
         <v>477</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>476</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>475</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>474</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>473</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>472</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>471</v>
       </c>
       <c r="T1" s="12"/>
       <c r="U1" s="12"/>
@@ -3535,41 +3553,41 @@
     </row>
     <row r="27" spans="1:27" ht="15.75" customHeight="1">
       <c r="A27" s="17" t="s">
-        <v>402</v>
+        <v>476</v>
       </c>
       <c r="B27" s="17">
         <f>VLOOKUP(A27,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>2</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>401</v>
+        <v>475</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>400</v>
+        <v>474</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="F27" s="20" t="s">
-        <v>399</v>
+      <c r="F27" s="17" t="s">
+        <v>473</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="H27" s="18" t="s">
-        <v>398</v>
+      <c r="H27" s="23" t="s">
+        <v>472</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>397</v>
+        <v>471</v>
       </c>
       <c r="J27" s="19">
-        <v>3661238568945</v>
+        <v>3410530223201</v>
       </c>
       <c r="K27" s="17">
-        <v>100019786</v>
+        <v>22120</v>
       </c>
       <c r="L27" s="17" t="s">
-        <v>188</v>
+        <v>322</v>
       </c>
       <c r="M27" s="17" t="s">
         <v>187</v>
@@ -3593,41 +3611,41 @@
     </row>
     <row r="28" spans="1:27" ht="15.75" customHeight="1">
       <c r="A28" s="17" t="s">
-        <v>214</v>
+        <v>402</v>
       </c>
       <c r="B28" s="17">
         <f>VLOOKUP(A28,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>2</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>213</v>
+        <v>401</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>212</v>
+        <v>400</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="F28" s="17" t="s">
-        <v>211</v>
+      <c r="F28" s="20" t="s">
+        <v>399</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>190</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>210</v>
+        <v>398</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>209</v>
+        <v>397</v>
       </c>
       <c r="J28" s="19">
-        <v>3546338714150</v>
+        <v>3661238568945</v>
       </c>
       <c r="K28" s="17">
-        <v>871415</v>
+        <v>100019786</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="M28" s="17" t="s">
         <v>187</v>
@@ -3651,41 +3669,41 @@
     </row>
     <row r="29" spans="1:27" ht="15.75" customHeight="1">
       <c r="A29" s="17" t="s">
-        <v>356</v>
+        <v>214</v>
       </c>
       <c r="B29" s="17">
         <f>VLOOKUP(A29,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>355</v>
+        <v>213</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>354</v>
+        <v>212</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>192</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>353</v>
+        <v>211</v>
       </c>
       <c r="G29" s="17" t="s">
         <v>190</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>352</v>
+        <v>210</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>351</v>
+        <v>209</v>
       </c>
       <c r="J29" s="19">
-        <v>3410531543254</v>
+        <v>3546338714150</v>
       </c>
       <c r="K29" s="17">
-        <v>154325</v>
+        <v>871415</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>322</v>
+        <v>208</v>
       </c>
       <c r="M29" s="17" t="s">
         <v>187</v>
@@ -3708,99 +3726,100 @@
       </c>
     </row>
     <row r="30" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A30" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="B30" s="6">
+      <c r="A30" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="B30" s="17">
         <f>VLOOKUP(A30,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>422</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>421</v>
-      </c>
-      <c r="E30" s="6" t="s">
+        <v>1.75</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="E30" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>420</v>
-      </c>
-      <c r="G30" s="6" t="s">
+      <c r="F30" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="G30" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="H30" s="8" t="s">
-        <v>419</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>418</v>
-      </c>
-      <c r="J30" s="16">
-        <v>3661238349124</v>
-      </c>
-      <c r="K30" s="6">
-        <v>100010305</v>
-      </c>
-      <c r="L30" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="M30" s="6" t="s">
+      <c r="H30" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="J30" s="19">
+        <v>3410531543254</v>
+      </c>
+      <c r="K30" s="17">
+        <v>154325</v>
+      </c>
+      <c r="L30" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="M30" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="N30" s="6">
+      <c r="N30" s="17">
         <v>621</v>
       </c>
-      <c r="O30" s="6" t="s">
+      <c r="O30" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="P30" s="6" t="s">
+      <c r="P30" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="Q30" s="6" t="s">
+      <c r="Q30" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="S30" s="6" t="s">
+      <c r="R30" s="17"/>
+      <c r="S30" s="17" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:27" ht="15.75" customHeight="1">
       <c r="A31" s="6" t="s">
-        <v>396</v>
+        <v>423</v>
       </c>
       <c r="B31" s="6">
         <f>VLOOKUP(A31,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>1</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>395</v>
+        <v>422</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>394</v>
+        <v>421</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>393</v>
+        <v>420</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>392</v>
+        <v>419</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>391</v>
+        <v>418</v>
       </c>
       <c r="J31" s="16">
-        <v>3410531531107</v>
+        <v>3661238349124</v>
       </c>
       <c r="K31" s="6">
-        <v>153110</v>
+        <v>100010305</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>322</v>
+        <v>188</v>
       </c>
       <c r="M31" s="6" t="s">
         <v>187</v>
@@ -3823,41 +3842,41 @@
     </row>
     <row r="32" spans="1:27" ht="15.75" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>291</v>
+        <v>396</v>
       </c>
       <c r="B32" s="6">
         <f>VLOOKUP(A32,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>1</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>290</v>
+        <v>395</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>289</v>
+        <v>394</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>288</v>
+        <v>393</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>287</v>
+        <v>392</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>286</v>
+        <v>391</v>
       </c>
       <c r="J32" s="16">
-        <v>3546332710479</v>
+        <v>3410531531107</v>
       </c>
       <c r="K32" s="6">
-        <v>271047</v>
+        <v>153110</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>208</v>
+        <v>322</v>
       </c>
       <c r="M32" s="6" t="s">
         <v>187</v>
@@ -3880,41 +3899,41 @@
     </row>
     <row r="33" spans="1:19" ht="15.75" customHeight="1">
       <c r="A33" s="6" t="s">
-        <v>237</v>
+        <v>291</v>
       </c>
       <c r="B33" s="6">
         <f>VLOOKUP(A33,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>1</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>236</v>
+        <v>290</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>235</v>
+        <v>289</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>234</v>
+        <v>288</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>233</v>
+        <v>287</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>232</v>
+        <v>286</v>
       </c>
       <c r="J33" s="16">
-        <v>3661238583719</v>
+        <v>3546332710479</v>
       </c>
       <c r="K33" s="6">
-        <v>7605040</v>
+        <v>271047</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="M33" s="6" t="s">
         <v>187</v>
@@ -3937,41 +3956,41 @@
     </row>
     <row r="34" spans="1:19" ht="15.75" customHeight="1">
       <c r="A34" s="6" t="s">
-        <v>470</v>
+        <v>237</v>
       </c>
       <c r="B34" s="6">
         <f>VLOOKUP(A34,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>469</v>
+        <v>236</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>468</v>
+        <v>235</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>467</v>
+        <v>234</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>466</v>
+        <v>233</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>465</v>
+        <v>232</v>
       </c>
       <c r="J34" s="16">
-        <v>3410530223300</v>
+        <v>3661238583719</v>
       </c>
       <c r="K34" s="6">
-        <v>22330</v>
+        <v>7605040</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>322</v>
+        <v>188</v>
       </c>
       <c r="M34" s="6" t="s">
         <v>187</v>
@@ -3994,38 +4013,38 @@
     </row>
     <row r="35" spans="1:19" ht="15.75" customHeight="1">
       <c r="A35" s="6" t="s">
-        <v>328</v>
+        <v>470</v>
       </c>
       <c r="B35" s="6">
         <f>VLOOKUP(A35,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>0.5</v>
+        <v>0.83</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>327</v>
+        <v>469</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>326</v>
+        <v>468</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F35" s="11" t="s">
-        <v>325</v>
+      <c r="F35" s="6" t="s">
+        <v>467</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H35" s="8" t="s">
-        <v>324</v>
+        <v>466</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>323</v>
+        <v>465</v>
       </c>
       <c r="J35" s="16">
-        <v>3410531554205</v>
+        <v>3410530223300</v>
       </c>
       <c r="K35" s="6">
-        <v>155420</v>
+        <v>22330</v>
       </c>
       <c r="L35" s="6" t="s">
         <v>322</v>
@@ -4051,41 +4070,41 @@
     </row>
     <row r="36" spans="1:19" ht="15.75" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>231</v>
+        <v>328</v>
       </c>
       <c r="B36" s="6">
         <f>VLOOKUP(A36,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0.5</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>230</v>
+        <v>327</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>326</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>229</v>
+      <c r="F36" s="11" t="s">
+        <v>325</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="H36" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>227</v>
+      <c r="H36" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>323</v>
       </c>
       <c r="J36" s="16">
-        <v>3661238583726</v>
+        <v>3410531554205</v>
       </c>
       <c r="K36" s="6">
-        <v>7605042</v>
+        <v>155420</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>188</v>
+        <v>322</v>
       </c>
       <c r="M36" s="6" t="s">
         <v>187</v>
@@ -4094,7 +4113,7 @@
         <v>621</v>
       </c>
       <c r="O36" s="6" t="s">
-        <v>226</v>
+        <v>186</v>
       </c>
       <c r="P36" s="6" t="s">
         <v>185</v>
@@ -4108,38 +4127,38 @@
     </row>
     <row r="37" spans="1:19" ht="15.75" customHeight="1">
       <c r="A37" s="6" t="s">
-        <v>429</v>
+        <v>231</v>
       </c>
       <c r="B37" s="6">
         <f>VLOOKUP(A37,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>428</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>427</v>
+        <v>70</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>230</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>426</v>
+        <v>229</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="H37" s="8" t="s">
-        <v>425</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>424</v>
+      <c r="H37" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>227</v>
       </c>
       <c r="J37" s="16">
-        <v>3661238349117</v>
+        <v>3661238583726</v>
       </c>
       <c r="K37" s="6">
-        <v>100010304</v>
+        <v>7605042</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>188</v>
@@ -4151,7 +4170,7 @@
         <v>621</v>
       </c>
       <c r="O37" s="6" t="s">
-        <v>186</v>
+        <v>226</v>
       </c>
       <c r="P37" s="6" t="s">
         <v>185</v>
@@ -4165,41 +4184,41 @@
     </row>
     <row r="38" spans="1:19" ht="15.75" customHeight="1">
       <c r="A38" s="6" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="B38" s="6">
         <f>VLOOKUP(A38,'cdes et cout'!A$2:E$52,5,FALSE)</f>
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>157</v>
+        <v>428</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="J38" s="16">
-        <v>3410530521253</v>
+        <v>3661238349117</v>
       </c>
       <c r="K38" s="6">
-        <v>52125</v>
+        <v>100010304</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>322</v>
+        <v>188</v>
       </c>
       <c r="M38" s="6" t="s">
         <v>187</v>
@@ -4222,41 +4241,41 @@
     </row>
     <row r="39" spans="1:19" ht="15.75" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>417</v>
+        <v>440</v>
       </c>
       <c r="B39" s="6">
         <f>VLOOKUP(A39,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>416</v>
+      <c r="C39" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>439</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>415</v>
+        <v>438</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="H39" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>413</v>
+      <c r="H39" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>436</v>
       </c>
       <c r="J39" s="16">
-        <v>3661238349131</v>
+        <v>3410530521253</v>
       </c>
       <c r="K39" s="6">
-        <v>100010306</v>
+        <v>52125</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>188</v>
+        <v>322</v>
       </c>
       <c r="M39" s="6" t="s">
         <v>187</v>
@@ -4273,44 +4292,44 @@
       <c r="Q39" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="S39" s="10" t="s">
+      <c r="S39" s="6" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:19" ht="15.75" customHeight="1">
       <c r="A40" s="6" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="B40" s="6">
         <f>VLOOKUP(A40,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>411</v>
+      <c r="C40" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>416</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="H40" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="I40" s="8" t="s">
-        <v>408</v>
+      <c r="H40" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>413</v>
       </c>
       <c r="J40" s="16">
-        <v>3661238568921</v>
+        <v>3661238349131</v>
       </c>
       <c r="K40" s="6">
-        <v>100019784</v>
+        <v>100010306</v>
       </c>
       <c r="L40" s="6" t="s">
         <v>188</v>
@@ -4330,44 +4349,44 @@
       <c r="Q40" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="S40" s="6" t="s">
+      <c r="S40" s="10" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:19" ht="15.75" customHeight="1">
       <c r="A41" s="6" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="B41" s="6">
         <f>VLOOKUP(A41,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="J41" s="16">
-        <v>3661238568938</v>
+        <v>3661238568921</v>
       </c>
       <c r="K41" s="6">
-        <v>100019785</v>
+        <v>100019784</v>
       </c>
       <c r="L41" s="6" t="s">
         <v>188</v>
@@ -4393,41 +4412,41 @@
     </row>
     <row r="42" spans="1:19" ht="15.75" customHeight="1">
       <c r="A42" s="6" t="s">
-        <v>333</v>
+        <v>407</v>
       </c>
       <c r="B42" s="6">
         <f>VLOOKUP(A42,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>332</v>
+        <v>406</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>331</v>
+        <v>405</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>330</v>
+        <v>404</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>329</v>
+        <v>403</v>
       </c>
       <c r="J42" s="16">
-        <v>3410531554106</v>
+        <v>3661238568938</v>
       </c>
       <c r="K42" s="6">
-        <v>155410</v>
+        <v>100019785</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>322</v>
+        <v>188</v>
       </c>
       <c r="M42" s="6" t="s">
         <v>187</v>
@@ -4450,41 +4469,41 @@
     </row>
     <row r="43" spans="1:19" ht="15.75" customHeight="1">
       <c r="A43" s="6" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="B43" s="6">
         <f>VLOOKUP(A43,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>107</v>
+        <v>153</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
       <c r="J43" s="16">
-        <v>3546332310389</v>
+        <v>3410531554106</v>
       </c>
       <c r="K43" s="6">
-        <v>231038</v>
+        <v>155410</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>208</v>
+        <v>322</v>
       </c>
       <c r="M43" s="6" t="s">
         <v>187</v>
@@ -4507,38 +4526,38 @@
     </row>
     <row r="44" spans="1:19" ht="15.75" customHeight="1">
       <c r="A44" s="6" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="B44" s="6">
         <f>VLOOKUP(A44,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="J44" s="16">
-        <v>3546332410980</v>
+        <v>3546332310389</v>
       </c>
       <c r="K44" s="6">
-        <v>241098</v>
+        <v>231038</v>
       </c>
       <c r="L44" s="6" t="s">
         <v>208</v>
@@ -4564,38 +4583,38 @@
     </row>
     <row r="45" spans="1:19" ht="15.75" customHeight="1">
       <c r="A45" s="6" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="B45" s="6">
         <f>VLOOKUP(A45,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>173</v>
+        <v>66</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>299</v>
+        <v>314</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>297</v>
+        <v>312</v>
       </c>
       <c r="J45" s="16">
-        <v>3546332610670</v>
+        <v>3546332410980</v>
       </c>
       <c r="K45" s="6">
-        <v>261067</v>
+        <v>241098</v>
       </c>
       <c r="L45" s="6" t="s">
         <v>208</v>
@@ -4621,38 +4640,38 @@
     </row>
     <row r="46" spans="1:19" ht="15.75" customHeight="1">
       <c r="A46" s="6" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="B46" s="6">
         <f>VLOOKUP(A46,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H46" s="8" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="J46" s="16">
-        <v>3546332631231</v>
+        <v>3546332610670</v>
       </c>
       <c r="K46" s="6">
-        <v>263123</v>
+        <v>261067</v>
       </c>
       <c r="L46" s="6" t="s">
         <v>208</v>
@@ -4678,38 +4697,38 @@
     </row>
     <row r="47" spans="1:19" ht="15.75" customHeight="1">
       <c r="A47" s="6" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="B47" s="6">
         <f>VLOOKUP(A47,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>212</v>
+        <v>295</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="J47" s="16">
-        <v>3546332710837</v>
+        <v>3546332631231</v>
       </c>
       <c r="K47" s="6">
-        <v>271083</v>
+        <v>263123</v>
       </c>
       <c r="L47" s="6" t="s">
         <v>208</v>
@@ -4735,38 +4754,38 @@
     </row>
     <row r="48" spans="1:19" ht="15.75" customHeight="1">
       <c r="A48" s="6" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="B48" s="6">
         <f>VLOOKUP(A48,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>280</v>
+        <v>212</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="J48" s="16">
-        <v>3546332810421</v>
+        <v>3546332710837</v>
       </c>
       <c r="K48" s="6">
-        <v>281042</v>
+        <v>271083</v>
       </c>
       <c r="L48" s="6" t="s">
         <v>208</v>
@@ -4792,38 +4811,38 @@
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1">
       <c r="A49" s="6" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="B49" s="6">
         <f>VLOOKUP(A49,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="J49" s="16">
-        <v>3546332810674</v>
+        <v>3546332810421</v>
       </c>
       <c r="K49" s="6">
-        <v>281067</v>
+        <v>281042</v>
       </c>
       <c r="L49" s="6" t="s">
         <v>208</v>
@@ -4849,38 +4868,38 @@
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1">
       <c r="A50" s="6" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="B50" s="6">
         <f>VLOOKUP(A50,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>125</v>
+        <v>161</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="J50" s="16">
-        <v>3546332831181</v>
+        <v>3546332810674</v>
       </c>
       <c r="K50" s="6">
-        <v>283118</v>
+        <v>281067</v>
       </c>
       <c r="L50" s="6" t="s">
         <v>208</v>
@@ -4906,38 +4925,38 @@
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1">
       <c r="A51" s="6" t="s">
-        <v>219</v>
+        <v>254</v>
       </c>
       <c r="B51" s="6">
         <f>VLOOKUP(A51,'cdes et cout'!A$2:E$52,5,FALSE)</f>
         <v>0</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>218</v>
+        <v>253</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>192</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>217</v>
+        <v>252</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>190</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>216</v>
+        <v>251</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>215</v>
+        <v>250</v>
       </c>
       <c r="J51" s="16">
-        <v>3546338614108</v>
+        <v>3546332831181</v>
       </c>
       <c r="K51" s="6">
-        <v>861410</v>
+        <v>283118</v>
       </c>
       <c r="L51" s="6" t="s">
         <v>208</v>
@@ -4960,16 +4979,72 @@
       <c r="S51" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="T51" s="7"/>
-      <c r="U51" s="7"/>
-      <c r="V51" s="7"/>
-      <c r="W51" s="7"/>
-      <c r="X51" s="7"/>
-      <c r="Y51" s="7"/>
-      <c r="Z51" s="7"/>
-      <c r="AA51" s="7"/>
-    </row>
-    <row r="52" spans="1:27" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="52" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A52" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B52" s="6">
+        <f>VLOOKUP(A52,'cdes et cout'!A$2:E$52,5,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="H52" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="I52" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="J52" s="16">
+        <v>3546338614108</v>
+      </c>
+      <c r="K52" s="6">
+        <v>861410</v>
+      </c>
+      <c r="L52" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="M52" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="N52" s="6">
+        <v>621</v>
+      </c>
+      <c r="O52" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="P52" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q52" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="S52" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="T52" s="7"/>
+      <c r="U52" s="7"/>
+      <c r="V52" s="7"/>
+      <c r="W52" s="7"/>
+      <c r="X52" s="7"/>
+      <c r="Y52" s="7"/>
+      <c r="Z52" s="7"/>
+      <c r="AA52" s="7"/>
+    </row>
     <row r="53" spans="1:27" ht="15.75" customHeight="1"/>
     <row r="54" spans="1:27" ht="15.75" customHeight="1"/>
     <row r="55" spans="1:27" ht="15.75" customHeight="1"/>
@@ -5917,111 +5992,114 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:S51" xr:uid="{5F843751-14C2-4F48-A3D1-34202082BFCD}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S51">
-      <sortCondition descending="1" ref="B2:B51"/>
+  <autoFilter ref="A1:S52" xr:uid="{5F843751-14C2-4F48-A3D1-34202082BFCD}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S52">
+      <sortCondition descending="1" ref="B2:B52"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="H34" r:id="rId1" xr:uid="{8F265B25-EDF8-47E6-A56D-648B10AAA291}"/>
-    <hyperlink ref="I34" r:id="rId2" xr:uid="{772FAAAD-31C4-4311-B5AB-00D8D42FD95C}"/>
-    <hyperlink ref="H14" r:id="rId3" xr:uid="{0601F08F-14C2-4EA8-B822-2CDF4698AE78}"/>
-    <hyperlink ref="I14" r:id="rId4" xr:uid="{262CFD04-3ADB-49C9-87CF-82297C1BDE16}"/>
-    <hyperlink ref="H12" r:id="rId5" xr:uid="{F84D323B-A869-4BD4-A35D-2E3C99D524FE}"/>
-    <hyperlink ref="I12" r:id="rId6" xr:uid="{8712264E-1946-426B-8648-27E8AF637FFB}"/>
-    <hyperlink ref="H18" r:id="rId7" xr:uid="{E7FB099C-1EA4-4530-A4CA-0D4044FCC560}"/>
-    <hyperlink ref="I18" r:id="rId8" xr:uid="{ECBD1FE0-91B4-4648-91F4-A13B65EDF8FD}"/>
-    <hyperlink ref="H5" r:id="rId9" xr:uid="{6A74B5BA-8EF1-42D6-9BE6-69B3580C19E3}"/>
-    <hyperlink ref="I5" r:id="rId10" xr:uid="{2048949F-8FAD-4C0F-A0D8-6F2E21D9FF20}"/>
-    <hyperlink ref="H38" r:id="rId11" xr:uid="{FF671DB2-F1DE-4A5F-A981-3B99BB398C8E}"/>
-    <hyperlink ref="I38" r:id="rId12" xr:uid="{54AA1E0D-9845-431A-A6B3-60B279DCA476}"/>
-    <hyperlink ref="H8" r:id="rId13" xr:uid="{B48B8A52-ECB7-4C10-A0FF-0FDB58298CD9}"/>
-    <hyperlink ref="I8" r:id="rId14" xr:uid="{F79786E9-9D1D-4DC5-8BBC-8DC9366FB347}"/>
-    <hyperlink ref="H37" r:id="rId15" xr:uid="{C6F7B82D-79A2-4CAE-9DBF-7A78BA2EE994}"/>
-    <hyperlink ref="I37" r:id="rId16" xr:uid="{3CAC15E0-A22A-4914-BCA8-3995022B8A9D}"/>
-    <hyperlink ref="H30" r:id="rId17" xr:uid="{BE80CC85-8952-4206-A6CE-D5EE149A8A51}"/>
-    <hyperlink ref="I30" r:id="rId18" xr:uid="{3DF18A14-3842-4EE7-838D-5B7007EF60AB}"/>
-    <hyperlink ref="H39" r:id="rId19" xr:uid="{B2AC5BB9-C667-4428-A602-3DD5760B92B4}"/>
-    <hyperlink ref="I39" r:id="rId20" xr:uid="{519FCFE8-2021-4F5E-9B52-0C55624CE5B1}"/>
-    <hyperlink ref="H40" r:id="rId21" xr:uid="{8C52E51A-84E8-4574-B7E6-66607B691481}"/>
-    <hyperlink ref="I40" r:id="rId22" xr:uid="{611DDBBB-F67C-443B-9DE8-15D176EF395A}"/>
-    <hyperlink ref="H41" r:id="rId23" xr:uid="{0588FF49-5A78-40D2-8714-F332862553A0}"/>
-    <hyperlink ref="I41" r:id="rId24" xr:uid="{2EDAFF60-3869-4FB3-94FA-C2CA11CB2602}"/>
-    <hyperlink ref="H27" r:id="rId25" xr:uid="{B95B938E-10B4-4A11-8BCA-E6B450153DF1}"/>
-    <hyperlink ref="I27" r:id="rId26" xr:uid="{6C8C2E0F-E162-4F06-A351-9DD2BA1E0116}"/>
-    <hyperlink ref="H31" r:id="rId27" xr:uid="{3BEDC9C8-7480-4517-B292-83DC8C4A8A0D}"/>
-    <hyperlink ref="I31" r:id="rId28" xr:uid="{01E86A13-A366-486F-B625-00B0F64382F2}"/>
-    <hyperlink ref="H16" r:id="rId29" xr:uid="{A02390C4-28A7-4129-A740-C2E37532AAF4}"/>
-    <hyperlink ref="I16" r:id="rId30" xr:uid="{F401772E-4D13-4E69-8345-52BB74433F38}"/>
-    <hyperlink ref="H7" r:id="rId31" xr:uid="{75199553-6D17-44D8-8A66-C4AE2131BD87}"/>
-    <hyperlink ref="I7" r:id="rId32" xr:uid="{890BBFD4-1471-43A2-A056-15E8F736FD4E}"/>
-    <hyperlink ref="H25" r:id="rId33" xr:uid="{2BD9953D-C1E7-4942-A62C-770EEFF28D76}"/>
-    <hyperlink ref="I25" r:id="rId34" xr:uid="{DC634B84-9A48-4EE2-B1F3-5D60C4815BC1}"/>
-    <hyperlink ref="H11" r:id="rId35" xr:uid="{CD963034-D20A-45F7-8273-9009DC597E76}"/>
-    <hyperlink ref="I11" r:id="rId36" xr:uid="{E177113C-5B3C-4A5F-B5E6-E9F6E8FA1B1D}"/>
-    <hyperlink ref="H19" r:id="rId37" xr:uid="{878F7461-702A-47DF-B955-5760FA9EFF1A}"/>
-    <hyperlink ref="I19" r:id="rId38" xr:uid="{BFFC4479-A5D2-420F-9075-6F4C889B61F9}"/>
-    <hyperlink ref="H17" r:id="rId39" xr:uid="{756EB775-EE14-4BBC-9B0C-4E1297FE42D1}"/>
-    <hyperlink ref="I17" r:id="rId40" xr:uid="{8BE6EF28-9646-41BC-8EA5-F8BC8A53BAA8}"/>
-    <hyperlink ref="H29" r:id="rId41" xr:uid="{5F4A6CC3-CCD5-4CF8-B333-8CAFFF58F2B7}"/>
-    <hyperlink ref="I29" r:id="rId42" xr:uid="{00FA8D30-9405-4EDF-9E91-F7F18721DA4B}"/>
-    <hyperlink ref="H2" r:id="rId43" xr:uid="{2A5E8E8C-F0B0-44FD-BAEB-B2C5DAF84D50}"/>
-    <hyperlink ref="I2" r:id="rId44" xr:uid="{D8BBCD78-271C-43B4-8B92-5F7F1E49E4E4}"/>
-    <hyperlink ref="H22" r:id="rId45" xr:uid="{D6FC507A-68E9-4763-AA79-3E87BC9253E8}"/>
-    <hyperlink ref="I22" r:id="rId46" xr:uid="{9A9544DA-4750-4CE1-89AE-F37C5E480315}"/>
-    <hyperlink ref="H3" r:id="rId47" xr:uid="{C9B382F8-D7E2-421C-91EB-8310CF808AB3}"/>
-    <hyperlink ref="I3" r:id="rId48" xr:uid="{8641A7C3-4048-4CDF-ABAD-25A50C9A6EAB}"/>
-    <hyperlink ref="H42" r:id="rId49" xr:uid="{800441B7-6446-4960-91EB-964CA344136D}"/>
-    <hyperlink ref="I42" r:id="rId50" xr:uid="{11C93C92-CB03-4282-BB1E-428C9A011CBE}"/>
-    <hyperlink ref="H35" r:id="rId51" xr:uid="{91D0E51F-5DE3-43C9-A6B8-D5BF1F3184AB}"/>
-    <hyperlink ref="I35" r:id="rId52" xr:uid="{90E6A90D-8248-4485-8D5D-01E5495C8CF3}"/>
-    <hyperlink ref="H43" r:id="rId53" xr:uid="{472FC637-15F3-4916-9782-D3C97325B98E}"/>
-    <hyperlink ref="I43" r:id="rId54" xr:uid="{2EE4C399-7DD8-421F-B37F-CC7A1800139C}"/>
-    <hyperlink ref="H44" r:id="rId55" xr:uid="{03456704-187C-4135-AD99-5281AA850205}"/>
-    <hyperlink ref="I44" r:id="rId56" xr:uid="{5B421C9F-78D3-4B0D-AFFF-1A8841A7CFC4}"/>
-    <hyperlink ref="H9" r:id="rId57" xr:uid="{A6B949BA-91A7-4F19-91D9-C27B88A58084}"/>
-    <hyperlink ref="I9" r:id="rId58" xr:uid="{50BCDB5C-AC05-428D-88CE-A9B0CEF73290}"/>
-    <hyperlink ref="H10" r:id="rId59" xr:uid="{ACF0AB68-E7D6-4155-A23A-DCD3B9BB0CDB}"/>
-    <hyperlink ref="I10" r:id="rId60" xr:uid="{B07F25F0-0A89-41A2-A279-5DFA9F5058D5}"/>
-    <hyperlink ref="H45" r:id="rId61" xr:uid="{182A0DA2-94FC-4100-A6E5-C223E4448AA5}"/>
-    <hyperlink ref="I45" r:id="rId62" xr:uid="{99C2E85F-C88C-4855-94BF-FFC3C4E5A0F9}"/>
-    <hyperlink ref="H46" r:id="rId63" xr:uid="{E3145210-EFF8-43C6-BDA4-4C5B4BA5D0D4}"/>
-    <hyperlink ref="I46" r:id="rId64" xr:uid="{A149C759-FA34-4714-BAA6-8930998887BC}"/>
-    <hyperlink ref="H32" r:id="rId65" xr:uid="{94DE6458-BBCF-42DC-9F2D-9984236B41E0}"/>
-    <hyperlink ref="I32" r:id="rId66" xr:uid="{C05331FA-B747-4A37-9B2F-5847A3B819B7}"/>
-    <hyperlink ref="H47" r:id="rId67" xr:uid="{765D3428-056A-49A5-8900-3A40B16E9BF8}"/>
-    <hyperlink ref="I47" r:id="rId68" xr:uid="{93D98F2E-3D2C-4606-9310-C8C41A7D41C7}"/>
-    <hyperlink ref="H48" r:id="rId69" xr:uid="{D8AA3DB6-9DBC-449F-A10D-E7EBEC12A453}"/>
-    <hyperlink ref="I48" r:id="rId70" xr:uid="{4DCC0358-CF9A-4E71-A1BA-C926A9048CE2}"/>
-    <hyperlink ref="H49" r:id="rId71" xr:uid="{A9C75572-1ACC-4C33-B416-7252D09928FA}"/>
-    <hyperlink ref="I49" r:id="rId72" xr:uid="{848F6251-0C9B-4D77-A569-453E702D1D9F}"/>
-    <hyperlink ref="H26" r:id="rId73" xr:uid="{0A555F60-5921-4BD2-8CB4-E3BF76A23F01}"/>
-    <hyperlink ref="I26" r:id="rId74" xr:uid="{94FB009D-6CB5-4A73-B31C-E7F49070311A}"/>
-    <hyperlink ref="H21" r:id="rId75" xr:uid="{6BF3C264-BD68-4437-8E7C-D84B122C5763}"/>
-    <hyperlink ref="I21" r:id="rId76" xr:uid="{254D2B03-ED1F-4468-B2F0-D1058756198A}"/>
-    <hyperlink ref="H23" r:id="rId77" xr:uid="{541331AF-4CFE-4458-AE54-EE44D847C4FD}"/>
-    <hyperlink ref="I23" r:id="rId78" xr:uid="{79F4E8EE-249E-4920-88BE-07DF6C3B0564}"/>
-    <hyperlink ref="H50" r:id="rId79" xr:uid="{DAEB5637-6945-493A-A843-9998179991B1}"/>
-    <hyperlink ref="I50" r:id="rId80" xr:uid="{FF26DAB0-F03A-4FBA-9598-075CE0666D13}"/>
-    <hyperlink ref="H24" r:id="rId81" xr:uid="{91A7B747-DB67-4060-8560-323DDF1923D2}"/>
-    <hyperlink ref="I24" r:id="rId82" xr:uid="{17074686-B527-478E-836F-3C8EB3B08C9C}"/>
-    <hyperlink ref="H6" r:id="rId83" xr:uid="{F78D3D90-EA33-400F-BE8E-76DBF64142BA}"/>
-    <hyperlink ref="I6" r:id="rId84" xr:uid="{77BB8E84-01A2-4E85-B992-64C45BA2934D}"/>
-    <hyperlink ref="H33" r:id="rId85" xr:uid="{FF95C280-4670-40A1-A612-C8D8B74CFBA1}"/>
-    <hyperlink ref="I33" r:id="rId86" xr:uid="{82265D57-FD4B-4A7B-8B75-52EC911B56AB}"/>
-    <hyperlink ref="H36" r:id="rId87" xr:uid="{1A01C6DB-9CBA-4A93-B436-C026328E928B}"/>
-    <hyperlink ref="I36" r:id="rId88" xr:uid="{84BC007C-86DD-4867-A9A0-B1923A6DCC2B}"/>
-    <hyperlink ref="H13" r:id="rId89" xr:uid="{BF64299C-2B33-4D98-A11C-DD41B908AA5B}"/>
-    <hyperlink ref="I13" r:id="rId90" xr:uid="{89324702-ADD1-43D8-9166-3237B9861112}"/>
-    <hyperlink ref="H51" r:id="rId91" xr:uid="{121E023A-10BB-4E86-ACA7-26736E4B8926}"/>
-    <hyperlink ref="I51" r:id="rId92" xr:uid="{F6AD4B58-435F-41F4-AD6D-0EE7698345B4}"/>
-    <hyperlink ref="H28" r:id="rId93" xr:uid="{FABCAC6F-0EA0-4D9A-B304-2D38ED3A684A}"/>
-    <hyperlink ref="I28" r:id="rId94" xr:uid="{C7309A15-7EDA-4400-ACAF-2666F1E1193F}"/>
-    <hyperlink ref="H15" r:id="rId95" xr:uid="{73065095-5BFB-47BE-BA84-CF4FF287680D}"/>
-    <hyperlink ref="I15" r:id="rId96" xr:uid="{10E084A1-80B5-4594-BC62-6956C26AB080}"/>
-    <hyperlink ref="H20" r:id="rId97" xr:uid="{BF18D7EE-A205-49E0-807B-B8EDE5723178}"/>
-    <hyperlink ref="I20" r:id="rId98" xr:uid="{B27CCBBD-F8AB-43A7-B92D-9588906D3D87}"/>
+    <hyperlink ref="H27" r:id="rId1" xr:uid="{99D8DFD9-6BE7-4C78-ABE2-95EE338B83D8}"/>
+    <hyperlink ref="I27" r:id="rId2" xr:uid="{E3FB3F43-4670-4E99-A48A-D044DBBE2C74}"/>
+    <hyperlink ref="H35" r:id="rId3" xr:uid="{8F265B25-EDF8-47E6-A56D-648B10AAA291}"/>
+    <hyperlink ref="I35" r:id="rId4" xr:uid="{772FAAAD-31C4-4311-B5AB-00D8D42FD95C}"/>
+    <hyperlink ref="H14" r:id="rId5" xr:uid="{0601F08F-14C2-4EA8-B822-2CDF4698AE78}"/>
+    <hyperlink ref="I14" r:id="rId6" xr:uid="{262CFD04-3ADB-49C9-87CF-82297C1BDE16}"/>
+    <hyperlink ref="H12" r:id="rId7" xr:uid="{F84D323B-A869-4BD4-A35D-2E3C99D524FE}"/>
+    <hyperlink ref="I12" r:id="rId8" xr:uid="{8712264E-1946-426B-8648-27E8AF637FFB}"/>
+    <hyperlink ref="H18" r:id="rId9" xr:uid="{E7FB099C-1EA4-4530-A4CA-0D4044FCC560}"/>
+    <hyperlink ref="I18" r:id="rId10" xr:uid="{ECBD1FE0-91B4-4648-91F4-A13B65EDF8FD}"/>
+    <hyperlink ref="H5" r:id="rId11" xr:uid="{6A74B5BA-8EF1-42D6-9BE6-69B3580C19E3}"/>
+    <hyperlink ref="I5" r:id="rId12" xr:uid="{2048949F-8FAD-4C0F-A0D8-6F2E21D9FF20}"/>
+    <hyperlink ref="H39" r:id="rId13" xr:uid="{FF671DB2-F1DE-4A5F-A981-3B99BB398C8E}"/>
+    <hyperlink ref="I39" r:id="rId14" xr:uid="{54AA1E0D-9845-431A-A6B3-60B279DCA476}"/>
+    <hyperlink ref="H8" r:id="rId15" xr:uid="{B48B8A52-ECB7-4C10-A0FF-0FDB58298CD9}"/>
+    <hyperlink ref="I8" r:id="rId16" xr:uid="{F79786E9-9D1D-4DC5-8BBC-8DC9366FB347}"/>
+    <hyperlink ref="H38" r:id="rId17" xr:uid="{C6F7B82D-79A2-4CAE-9DBF-7A78BA2EE994}"/>
+    <hyperlink ref="I38" r:id="rId18" xr:uid="{3CAC15E0-A22A-4914-BCA8-3995022B8A9D}"/>
+    <hyperlink ref="H31" r:id="rId19" xr:uid="{BE80CC85-8952-4206-A6CE-D5EE149A8A51}"/>
+    <hyperlink ref="I31" r:id="rId20" xr:uid="{3DF18A14-3842-4EE7-838D-5B7007EF60AB}"/>
+    <hyperlink ref="H40" r:id="rId21" xr:uid="{B2AC5BB9-C667-4428-A602-3DD5760B92B4}"/>
+    <hyperlink ref="I40" r:id="rId22" xr:uid="{519FCFE8-2021-4F5E-9B52-0C55624CE5B1}"/>
+    <hyperlink ref="H41" r:id="rId23" xr:uid="{8C52E51A-84E8-4574-B7E6-66607B691481}"/>
+    <hyperlink ref="I41" r:id="rId24" xr:uid="{611DDBBB-F67C-443B-9DE8-15D176EF395A}"/>
+    <hyperlink ref="H42" r:id="rId25" xr:uid="{0588FF49-5A78-40D2-8714-F332862553A0}"/>
+    <hyperlink ref="I42" r:id="rId26" xr:uid="{2EDAFF60-3869-4FB3-94FA-C2CA11CB2602}"/>
+    <hyperlink ref="H28" r:id="rId27" xr:uid="{B95B938E-10B4-4A11-8BCA-E6B450153DF1}"/>
+    <hyperlink ref="I28" r:id="rId28" xr:uid="{6C8C2E0F-E162-4F06-A351-9DD2BA1E0116}"/>
+    <hyperlink ref="H32" r:id="rId29" xr:uid="{3BEDC9C8-7480-4517-B292-83DC8C4A8A0D}"/>
+    <hyperlink ref="I32" r:id="rId30" xr:uid="{01E86A13-A366-486F-B625-00B0F64382F2}"/>
+    <hyperlink ref="H16" r:id="rId31" xr:uid="{A02390C4-28A7-4129-A740-C2E37532AAF4}"/>
+    <hyperlink ref="I16" r:id="rId32" xr:uid="{F401772E-4D13-4E69-8345-52BB74433F38}"/>
+    <hyperlink ref="H7" r:id="rId33" xr:uid="{75199553-6D17-44D8-8A66-C4AE2131BD87}"/>
+    <hyperlink ref="I7" r:id="rId34" xr:uid="{890BBFD4-1471-43A2-A056-15E8F736FD4E}"/>
+    <hyperlink ref="H25" r:id="rId35" xr:uid="{2BD9953D-C1E7-4942-A62C-770EEFF28D76}"/>
+    <hyperlink ref="I25" r:id="rId36" xr:uid="{DC634B84-9A48-4EE2-B1F3-5D60C4815BC1}"/>
+    <hyperlink ref="H11" r:id="rId37" xr:uid="{CD963034-D20A-45F7-8273-9009DC597E76}"/>
+    <hyperlink ref="I11" r:id="rId38" xr:uid="{E177113C-5B3C-4A5F-B5E6-E9F6E8FA1B1D}"/>
+    <hyperlink ref="H19" r:id="rId39" xr:uid="{878F7461-702A-47DF-B955-5760FA9EFF1A}"/>
+    <hyperlink ref="I19" r:id="rId40" xr:uid="{BFFC4479-A5D2-420F-9075-6F4C889B61F9}"/>
+    <hyperlink ref="H17" r:id="rId41" xr:uid="{756EB775-EE14-4BBC-9B0C-4E1297FE42D1}"/>
+    <hyperlink ref="I17" r:id="rId42" xr:uid="{8BE6EF28-9646-41BC-8EA5-F8BC8A53BAA8}"/>
+    <hyperlink ref="H30" r:id="rId43" xr:uid="{5F4A6CC3-CCD5-4CF8-B333-8CAFFF58F2B7}"/>
+    <hyperlink ref="I30" r:id="rId44" xr:uid="{00FA8D30-9405-4EDF-9E91-F7F18721DA4B}"/>
+    <hyperlink ref="H2" r:id="rId45" xr:uid="{2A5E8E8C-F0B0-44FD-BAEB-B2C5DAF84D50}"/>
+    <hyperlink ref="I2" r:id="rId46" xr:uid="{D8BBCD78-271C-43B4-8B92-5F7F1E49E4E4}"/>
+    <hyperlink ref="H22" r:id="rId47" xr:uid="{D6FC507A-68E9-4763-AA79-3E87BC9253E8}"/>
+    <hyperlink ref="I22" r:id="rId48" xr:uid="{9A9544DA-4750-4CE1-89AE-F37C5E480315}"/>
+    <hyperlink ref="H3" r:id="rId49" xr:uid="{C9B382F8-D7E2-421C-91EB-8310CF808AB3}"/>
+    <hyperlink ref="I3" r:id="rId50" xr:uid="{8641A7C3-4048-4CDF-ABAD-25A50C9A6EAB}"/>
+    <hyperlink ref="H43" r:id="rId51" xr:uid="{800441B7-6446-4960-91EB-964CA344136D}"/>
+    <hyperlink ref="I43" r:id="rId52" xr:uid="{11C93C92-CB03-4282-BB1E-428C9A011CBE}"/>
+    <hyperlink ref="H36" r:id="rId53" xr:uid="{91D0E51F-5DE3-43C9-A6B8-D5BF1F3184AB}"/>
+    <hyperlink ref="I36" r:id="rId54" xr:uid="{90E6A90D-8248-4485-8D5D-01E5495C8CF3}"/>
+    <hyperlink ref="H44" r:id="rId55" xr:uid="{472FC637-15F3-4916-9782-D3C97325B98E}"/>
+    <hyperlink ref="I44" r:id="rId56" xr:uid="{2EE4C399-7DD8-421F-B37F-CC7A1800139C}"/>
+    <hyperlink ref="H45" r:id="rId57" xr:uid="{03456704-187C-4135-AD99-5281AA850205}"/>
+    <hyperlink ref="I45" r:id="rId58" xr:uid="{5B421C9F-78D3-4B0D-AFFF-1A8841A7CFC4}"/>
+    <hyperlink ref="H9" r:id="rId59" xr:uid="{A6B949BA-91A7-4F19-91D9-C27B88A58084}"/>
+    <hyperlink ref="I9" r:id="rId60" xr:uid="{50BCDB5C-AC05-428D-88CE-A9B0CEF73290}"/>
+    <hyperlink ref="H10" r:id="rId61" xr:uid="{ACF0AB68-E7D6-4155-A23A-DCD3B9BB0CDB}"/>
+    <hyperlink ref="I10" r:id="rId62" xr:uid="{B07F25F0-0A89-41A2-A279-5DFA9F5058D5}"/>
+    <hyperlink ref="H46" r:id="rId63" xr:uid="{182A0DA2-94FC-4100-A6E5-C223E4448AA5}"/>
+    <hyperlink ref="I46" r:id="rId64" xr:uid="{99C2E85F-C88C-4855-94BF-FFC3C4E5A0F9}"/>
+    <hyperlink ref="H47" r:id="rId65" xr:uid="{E3145210-EFF8-43C6-BDA4-4C5B4BA5D0D4}"/>
+    <hyperlink ref="I47" r:id="rId66" xr:uid="{A149C759-FA34-4714-BAA6-8930998887BC}"/>
+    <hyperlink ref="H33" r:id="rId67" xr:uid="{94DE6458-BBCF-42DC-9F2D-9984236B41E0}"/>
+    <hyperlink ref="I33" r:id="rId68" xr:uid="{C05331FA-B747-4A37-9B2F-5847A3B819B7}"/>
+    <hyperlink ref="H48" r:id="rId69" xr:uid="{765D3428-056A-49A5-8900-3A40B16E9BF8}"/>
+    <hyperlink ref="I48" r:id="rId70" xr:uid="{93D98F2E-3D2C-4606-9310-C8C41A7D41C7}"/>
+    <hyperlink ref="H49" r:id="rId71" xr:uid="{D8AA3DB6-9DBC-449F-A10D-E7EBEC12A453}"/>
+    <hyperlink ref="I49" r:id="rId72" xr:uid="{4DCC0358-CF9A-4E71-A1BA-C926A9048CE2}"/>
+    <hyperlink ref="H50" r:id="rId73" xr:uid="{A9C75572-1ACC-4C33-B416-7252D09928FA}"/>
+    <hyperlink ref="I50" r:id="rId74" xr:uid="{848F6251-0C9B-4D77-A569-453E702D1D9F}"/>
+    <hyperlink ref="H26" r:id="rId75" xr:uid="{0A555F60-5921-4BD2-8CB4-E3BF76A23F01}"/>
+    <hyperlink ref="I26" r:id="rId76" xr:uid="{94FB009D-6CB5-4A73-B31C-E7F49070311A}"/>
+    <hyperlink ref="H21" r:id="rId77" xr:uid="{6BF3C264-BD68-4437-8E7C-D84B122C5763}"/>
+    <hyperlink ref="I21" r:id="rId78" xr:uid="{254D2B03-ED1F-4468-B2F0-D1058756198A}"/>
+    <hyperlink ref="H23" r:id="rId79" xr:uid="{541331AF-4CFE-4458-AE54-EE44D847C4FD}"/>
+    <hyperlink ref="I23" r:id="rId80" xr:uid="{79F4E8EE-249E-4920-88BE-07DF6C3B0564}"/>
+    <hyperlink ref="H51" r:id="rId81" xr:uid="{DAEB5637-6945-493A-A843-9998179991B1}"/>
+    <hyperlink ref="I51" r:id="rId82" xr:uid="{FF26DAB0-F03A-4FBA-9598-075CE0666D13}"/>
+    <hyperlink ref="H24" r:id="rId83" xr:uid="{91A7B747-DB67-4060-8560-323DDF1923D2}"/>
+    <hyperlink ref="I24" r:id="rId84" xr:uid="{17074686-B527-478E-836F-3C8EB3B08C9C}"/>
+    <hyperlink ref="H6" r:id="rId85" xr:uid="{F78D3D90-EA33-400F-BE8E-76DBF64142BA}"/>
+    <hyperlink ref="I6" r:id="rId86" xr:uid="{77BB8E84-01A2-4E85-B992-64C45BA2934D}"/>
+    <hyperlink ref="H34" r:id="rId87" xr:uid="{FF95C280-4670-40A1-A612-C8D8B74CFBA1}"/>
+    <hyperlink ref="I34" r:id="rId88" xr:uid="{82265D57-FD4B-4A7B-8B75-52EC911B56AB}"/>
+    <hyperlink ref="H37" r:id="rId89" xr:uid="{1A01C6DB-9CBA-4A93-B436-C026328E928B}"/>
+    <hyperlink ref="I37" r:id="rId90" xr:uid="{84BC007C-86DD-4867-A9A0-B1923A6DCC2B}"/>
+    <hyperlink ref="H13" r:id="rId91" xr:uid="{BF64299C-2B33-4D98-A11C-DD41B908AA5B}"/>
+    <hyperlink ref="I13" r:id="rId92" xr:uid="{89324702-ADD1-43D8-9166-3237B9861112}"/>
+    <hyperlink ref="H52" r:id="rId93" xr:uid="{121E023A-10BB-4E86-ACA7-26736E4B8926}"/>
+    <hyperlink ref="I52" r:id="rId94" xr:uid="{F6AD4B58-435F-41F4-AD6D-0EE7698345B4}"/>
+    <hyperlink ref="H29" r:id="rId95" xr:uid="{FABCAC6F-0EA0-4D9A-B304-2D38ED3A684A}"/>
+    <hyperlink ref="I29" r:id="rId96" xr:uid="{C7309A15-7EDA-4400-ACAF-2666F1E1193F}"/>
+    <hyperlink ref="H15" r:id="rId97" xr:uid="{73065095-5BFB-47BE-BA84-CF4FF287680D}"/>
+    <hyperlink ref="I15" r:id="rId98" xr:uid="{10E084A1-80B5-4594-BC62-6956C26AB080}"/>
+    <hyperlink ref="H20" r:id="rId99" xr:uid="{BF18D7EE-A205-49E0-807B-B8EDE5723178}"/>
+    <hyperlink ref="I20" r:id="rId100" xr:uid="{B27CCBBD-F8AB-43A7-B92D-9588906D3D87}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -6037,9 +6115,9 @@
       <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="11.41796875" style="2"/>
+    <col min="3" max="3" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">

</xml_diff>